<commit_message>
added forms to excel import / select form
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2129AF10-DD56-4542-BEAD-6DFBB2B952BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB4E1C-1A4E-714B-BE74-B5F259CC580B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="17" r:id="rId1"/>
+    <sheet name="forms" sheetId="18" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Username</t>
   </si>
@@ -112,13 +113,25 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>{"formId":"address-form","elems":[{"ident":"TITLE-3549","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"HUGE"}]},"value":"","required":false,"layoutWide":"SIXTEEN","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":false,"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":true,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+  </si>
+  <si>
+    <t>address-form</t>
+  </si>
+  <si>
+    <t>Form Id</t>
+  </si>
+  <si>
+    <t>Content</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +147,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +165,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,9 +187,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB2D3C8-E974-204A-9043-47C23044568C}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -588,4 +616,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73630E78-9998-5148-A4F5-0F74AED6B7AF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="92.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added data to excel import
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDB4E1C-1A4E-714B-BE74-B5F259CC580B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EFB9D0-643E-FB49-94BC-CEEDC96E748E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="17" r:id="rId1"/>
     <sheet name="forms" sheetId="18" r:id="rId2"/>
+    <sheet name="data" sheetId="19" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Username</t>
   </si>
@@ -115,16 +116,25 @@
     <t>admin</t>
   </si>
   <si>
-    <t>{"formId":"address-form","elems":[{"ident":"TITLE-3549","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"HUGE"}]},"value":"","required":false,"layoutWide":"SIXTEEN","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":false,"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":true,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
-  </si>
-  <si>
     <t>address-form</t>
   </si>
   <si>
-    <t>Form Id</t>
-  </si>
-  <si>
     <t>Content</t>
+  </si>
+  <si>
+    <t>Form Id (ident)</t>
+  </si>
+  <si>
+    <t>Data Id (ident)</t>
+  </si>
+  <si>
+    <t>address-data</t>
+  </si>
+  <si>
+    <t>{"ident":"address-data","structure":{"value":{"street":{"DataString":{"value":"Sonnenweg"}},"number":{"DataString":{"value":"23a"}},"postcode":{"DataNumber":{"value":6414}},"city":{"DataString":{"value":"Oberarth"}}}}}</t>
+  </si>
+  <si>
+    <t>{"ident":"address-form","elems":[{"ident":"TITLE-3549","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"HUGE"}]},"value":"","required":false,"layoutWide":"SIXTEEN","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":false,"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":true,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
   </si>
 </sst>
 </file>
@@ -623,11 +633,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="92.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -636,15 +647,50 @@
         <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED31875-2B24-DD47-B72C-6F638FA3F984}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="170" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="92.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding mapping to persist and excel / working with data/ elems
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EFB9D0-643E-FB49-94BC-CEEDC96E748E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC73A37D-DA1B-2846-8F50-72D880F7D428}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="17" r:id="rId1"/>
     <sheet name="forms" sheetId="18" r:id="rId2"/>
     <sheet name="data" sheetId="19" r:id="rId3"/>
+    <sheet name="mappings" sheetId="20" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Username</t>
   </si>
@@ -134,7 +135,16 @@
     <t>{"ident":"address-data","structure":{"value":{"street":{"DataString":{"value":"Sonnenweg"}},"number":{"DataString":{"value":"23a"}},"postcode":{"DataNumber":{"value":6414}},"city":{"DataString":{"value":"Oberarth"}}}}}</t>
   </si>
   <si>
-    <t>{"ident":"address-form","elems":[{"ident":"TITLE-3549","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"HUGE"}]},"value":"","required":false,"layoutWide":"SIXTEEN","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":false,"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":true,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+    <t>{"ident":"address-form","elems":[{"ident":"TITLE-60664","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"HUGE"}]},"value":"","required":false,"inline":false,"readOnly":true,"layoutWide":"SIXTEEN","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":false,"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+  </si>
+  <si>
+    <t>Mapping Id (ident)</t>
+  </si>
+  <si>
+    <t>address-mapping</t>
+  </si>
+  <si>
+    <t>{"ident":"address-mapping","formIdent":"address-form","dataIdent":"address-data","mappings":[{"formIdent":"TEXTFIELD-42","dataIdent":"street"},{"formIdent":"TEXTFIELD-14911"},{"formIdent":"TEXTFIELD-33671"},{"formIdent":"TEXTFIELD-90871"}]}</t>
   </si>
 </sst>
 </file>
@@ -632,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73630E78-9998-5148-A4F5-0F74AED6B7AF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
+    <sheetView zoomScale="170" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -668,7 +678,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="170" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -696,4 +706,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A6BC9-3416-B348-8790-05B6BEA43B74}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactoring client moved form stuff
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC73A37D-DA1B-2846-8F50-72D880F7D428}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71165B67-444B-7048-A93A-067F0C0A1EFA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
     <t>address-mapping</t>
   </si>
   <si>
-    <t>{"ident":"address-mapping","formIdent":"address-form","dataIdent":"address-data","mappings":[{"formIdent":"TEXTFIELD-42","dataIdent":"street"},{"formIdent":"TEXTFIELD-14911"},{"formIdent":"TEXTFIELD-33671"},{"formIdent":"TEXTFIELD-90871"}]}</t>
+    <t>{"ident":"address-mapping","formIdent":"address-form","dataIdent":"address-data","mappings":[{"formIdent":"TEXTFIELD-42","dataIdent":"street"},{"formIdent":"TEXTFIELD-14911","dataIdent":"number"},{"formIdent":"TEXTFIELD-33671","dataIdent":"postcode"},{"formIdent":"TEXTFIELD-90871","dataIdent":"city"}]}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
refactoring data models for forms
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71165B67-444B-7048-A93A-067F0C0A1EFA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B7F0C8-433C-0A41-8633-905EBCB77773}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="17" r:id="rId1"/>
@@ -642,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73630E78-9998-5148-A4F5-0F74AED6B7AF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="170" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -712,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A6BC9-3416-B348-8790-05B6BEA43B74}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+    <sheetView zoomScale="163" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes after BaseElementDiv.scala refactoring
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B7F0C8-433C-0A41-8633-905EBCB77773}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F6EEA9-3406-E741-AC78-749D2EDD49D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>{"ident":"address-data","structure":{"value":{"street":{"DataString":{"value":"Sonnenweg"}},"number":{"DataString":{"value":"23a"}},"postcode":{"DataNumber":{"value":6414}},"city":{"DataString":{"value":"Oberarth"}}}}}</t>
   </si>
   <si>
-    <t>{"ident":"address-form","elems":[{"ident":"TITLE-60664","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"HUGE"}]},"value":"","required":false,"inline":false,"readOnly":true,"layoutWide":"SIXTEEN","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":false,"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"hasEntries":false,"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
-  </si>
-  <si>
     <t>Mapping Id (ident)</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>{"ident":"address-mapping","formIdent":"address-form","dataIdent":"address-data","mappings":[{"formIdent":"TEXTFIELD-42","dataIdent":"street"},{"formIdent":"TEXTFIELD-14911","dataIdent":"number"},{"formIdent":"TEXTFIELD-33671","dataIdent":"postcode"},{"formIdent":"TEXTFIELD-90871","dataIdent":"city"}]}</t>
+  </si>
+  <si>
+    <t>{"ident":"address-form","elems":[{"ident":"TITLE-60664","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"HUGE"}]},"value":"","required":false,"inline":false,"readOnly":true,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"hasValidations":false,"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"Sonnenweg","required":true,"inline":false,"readOnly":true,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"23a","required":false,"inline":false,"readOnly":true,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"6414","required":false,"inline":false,"readOnly":true,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[]},"value":"Oberarth","required":false,"inline":false,"readOnly":true,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"hasValidations":true,"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>28</v>
@@ -731,10 +731,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes trying create a Form
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF56379-2A51-FA44-8CD0-6525411D299F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BEA726-03F5-5B4B-B18B-FA36B4D3D6FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>{"ident":"address-form","elems":[{"ident":"TITLE-60664","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Sonnenweg","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"23a","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"number"}]},"value":"6414","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":9999}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Oberarth","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+  </si>
+  <si>
+    <t>send-email</t>
+  </si>
+  <si>
+    <t>{"ident":"send-email","elems":[{"ident":"ELEM-84079","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Send Email Task","DE":"Send Email Task"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"smtpConfig","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"SMTP Configuration","DE":"SMTP Konfiguration"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"default","required":false,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"subject","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Subject","DE":"Betreff"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"I18N Email Test-Subject: {{mail.info.subject}}!","required":true,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"content","elementType":"TEXTAREA","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Content","DE":"Inhalt"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"Guten Tag\n\nDies ist ein Test Email.\n\nFreundliche Grüsse\n\nBPF-Team","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"from","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"From (Sender)","DE":"Von (Sender)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Email Address of the Sender.","DE":"Email Adresse des Senders."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"sender@finnova.ch","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":true,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"to","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"To (Recipients)","DE":"To (Empfänger)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Semicolon separated list of all recipient's email addresses .","DE":"Strichpunkt getrennte Liste aller Email-Adressen der Empfänger."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"hans.muster@test.com; vreny.mueller@test.com","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"ELEM-73603","elementType":"DIVIDER","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Additional Attributes for HTML Emails","DE":"Weitere Werte für die HTML Emails"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"templName","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Name","DE":"Template Name"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"The name of the HTML Template File.","DE":"Der Name der HTML Template Date."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"info_mail.html","required":false,"inline":false,"readOnly":false,"layoutWide":"TEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"language","elementType":"DROPDOWN","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Language","DE":"Sprache"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"CLEARABLE","value":"false"}]},"value":"DE","required":false,"inline":false,"readOnly":false,"layoutWide":"SIX","elemEntries":{"entries":[{"key":"DE","label":{"textType":"LABEL","texts":{"EN":"German","DE":"Deutsch"}},"ident":"ENTRY-3318"},{"key":"EN","label":{"textType":"LABEL","texts":{"EN":"English","DE":"Englisch"}},"ident":"ENTRY-3546"}]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"ELEM-54758","elementType":"TEXTAREA","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Parameters","DE":"Template Parameter"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Parameters as a Map that are used in the Template.","DE":"Ein JSON-Objekt, mit den Parameter, welche dem Template mitgegeben werden."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"{\n \"header\": \"Finnova rocks\",\n \"greeting\": \"Dear Mister President\",\n \"content\": \"Lory Logsi Dogsi Email content with Link: link:nextTask\",\n \"footer\": \"visit us!\",\n \"nextTask\": \"Go to next Task.\",\n \"nextTaskLink\": \"link:nextTask\",\n \"startInstance\": \"Start new Process Instance\",\n \"startInstanceLink\": \"link:startInstance\"\n }","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
   </si>
 </sst>
 </file>
@@ -641,10 +647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73630E78-9998-5148-A4F5-0F74AED6B7AF}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="170" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -667,6 +673,14 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added automatic creation of Data from Form
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BEA726-03F5-5B4B-B18B-FA36B4D3D6FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CA8ECA-4E63-7B43-8EBC-1F30BF3DCE36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,13 +145,13 @@
     <t>{"ident":"address-mapping","formIdent":"address-form","dataIdent":"address-data","mappings":[{"formIdent":"TEXTFIELD-42","dataIdent":"street"},{"formIdent":"TEXTFIELD-14911","dataIdent":"number"},{"formIdent":"TEXTFIELD-33671","dataIdent":"postcode"},{"formIdent":"TEXTFIELD-90871","dataIdent":"city"}]}</t>
   </si>
   <si>
-    <t>{"ident":"address-form","elems":[{"ident":"TITLE-60664","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[]}},{"ident":"TEXTFIELD-42","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Sonnenweg","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-14911","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"23a","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-33671","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"number"}]},"value":"6414","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":9999}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"TEXTFIELD-90871","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Oberarth","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
-  </si>
-  <si>
     <t>send-email</t>
   </si>
   <si>
-    <t>{"ident":"send-email","elems":[{"ident":"ELEM-84079","elementType":"TITLE","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Send Email Task","DE":"Send Email Task"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"smtpConfig","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"SMTP Configuration","DE":"SMTP Konfiguration"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"default","required":false,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"subject","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Subject","DE":"Betreff"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"I18N Email Test-Subject: {{mail.info.subject}}!","required":true,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"content","elementType":"TEXTAREA","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Content","DE":"Inhalt"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"Guten Tag\n\nDies ist ein Test Email.\n\nFreundliche Grüsse\n\nBPF-Team","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"from","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"From (Sender)","DE":"Von (Sender)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Email Address of the Sender.","DE":"Email Adresse des Senders."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"sender@finnova.ch","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":true,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"to","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"To (Recipients)","DE":"To (Empfänger)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Semicolon separated list of all recipient's email addresses .","DE":"Strichpunkt getrennte Liste aller Email-Adressen der Empfänger."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"hans.muster@test.com; vreny.mueller@test.com","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"ELEM-73603","elementType":"DIVIDER","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Additional Attributes for HTML Emails","DE":"Weitere Werte für die HTML Emails"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"templName","elementType":"TEXTFIELD","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Name","DE":"Template Name"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"The name of the HTML Template File.","DE":"Der Name der HTML Template Date."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"info_mail.html","required":false,"inline":false,"readOnly":false,"layoutWide":"TEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"language","elementType":"DROPDOWN","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Language","DE":"Sprache"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"CLEARABLE","value":"false"}]},"value":"DE","required":false,"inline":false,"readOnly":false,"layoutWide":"SIX","elemEntries":{"entries":[{"key":"DE","label":{"textType":"LABEL","texts":{"EN":"German","DE":"Deutsch"}},"ident":"ENTRY-3318"},{"key":"EN","label":{"textType":"LABEL","texts":{"EN":"English","DE":"Englisch"}},"ident":"ENTRY-3546"}]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"ELEM-54758","elementType":"TEXTAREA","dataType":"STRING","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Parameters","DE":"Template Parameter"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Parameters as a Map that are used in the Template.","DE":"Ein JSON-Objekt, mit den Parameter, welche dem Template mitgegeben werden."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"{\n \"header\": \"Finnova rocks\",\n \"greeting\": \"Dear Mister President\",\n \"content\": \"Lory Logsi Dogsi Email content with Link: link:nextTask\",\n \"footer\": \"visit us!\",\n \"nextTask\": \"Go to next Task.\",\n \"nextTaskLink\": \"link:nextTask\",\n \"startInstance\": \"Start new Process Instance\",\n \"startInstanceLink\": \"link:startInstance\"\n }","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+    <t>{"ident":"send-email","elems":[{"ident":"ELEM-84079","elementType":"TITLE","texts":{"label":{"textType":"LABEL","texts":{"EN":"Send Email Task","DE":"Send Email Task"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"smtpConfig","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"SMTP Configuration","DE":"SMTP Konfiguration"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"default","required":false,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"subject","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Subject","DE":"Betreff"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"I18N Email Test-Subject: {{mail.info.subject}}!","required":true,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"content","elementType":"TEXTAREA","texts":{"label":{"textType":"LABEL","texts":{"EN":"Content","DE":"Inhalt"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"Guten Tag\n\nDies ist ein Test Email.\n\nFreundliche Grüsse\n\nBPF-Team","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"from","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"From (Sender)","DE":"Von (Sender)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Email Address of the Sender.","DE":"Email Adresse des Senders."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"sender@finnova.ch","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":true,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"to","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"To (Recipients)","DE":"To (Empfänger)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Semicolon separated list of all recipient's email addresses .","DE":"Strichpunkt getrennte Liste aller Email-Adressen der Empfänger."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"hans.muster@test.com; vreny.mueller@test.com","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"ELEM-73603","elementType":"DIVIDER","texts":{"label":{"textType":"LABEL","texts":{"EN":"Additional Attributes for HTML Emails","DE":"Weitere Werte für die HTML Emails"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"templName","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Name","DE":"Template Name"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"The name of the HTML Template File.","DE":"Der Name der HTML Template Date."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"info_mail.html","required":false,"inline":false,"readOnly":false,"layoutWide":"TEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"language","elementType":"DROPDOWN","texts":{"label":{"textType":"LABEL","texts":{"EN":"Language","DE":"Sprache"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"CLEARABLE","value":"false"}]},"value":"DE","required":false,"inline":false,"readOnly":false,"layoutWide":"SIX","elemEntries":{"entries":[{"key":"DE","label":{"textType":"LABEL","texts":{"EN":"German","DE":"Deutsch"}},"ident":"ENTRY-3318"},{"key":"EN","label":{"textType":"LABEL","texts":{"EN":"English","DE":"Englisch"}},"ident":"ENTRY-3546"}]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"templParams","elementType":"TEXTAREA","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Parameters","DE":"Template Parameter"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Parameters as a Map that are used in the Template.","DE":"Ein JSON-Objekt, mit den Parameter, welche dem Template mitgegeben werden."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"{\n \"header\": \"Finnova rocks\",\n \"greeting\": \"Dear Mister President\",\n \"content\": \"Lory Logsi Dogsi Email content with Link: link:nextTask\",\n \"footer\": \"visit us!\",\n \"nextTask\": \"Go to next Task.\",\n \"nextTaskLink\": \"link:nextTask\",\n \"startInstance\": \"Start new Process Instance\",\n \"startInstanceLink\": \"link:startInstance\"\n }","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+  </si>
+  <si>
+    <t>{"ident":"address-form","elems":[{"ident":"TITLE-60664","elementType":"TITLE","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[]}},{"ident":"street","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Sonnenweg","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"number","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"23a","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"postcode","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"number"}]},"value":"6414","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":9999}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"town","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Oberarth","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
   </si>
 </sst>
 </file>
@@ -650,13 +650,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="170" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="92.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -672,15 +672,15 @@
         <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added automatic creation of Mapping from Form and Data
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CA8ECA-4E63-7B43-8EBC-1F30BF3DCE36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93256BC-626F-964D-87B1-A94952765F0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="17" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>address-form</t>
-  </si>
-  <si>
     <t>Content</t>
   </si>
   <si>
@@ -133,25 +130,28 @@
     <t>address-data</t>
   </si>
   <si>
-    <t>{"ident":"address-data","structure":{"value":{"street":{"DataString":{"value":"Sonnenweg"}},"number":{"DataString":{"value":"23a"}},"postcode":{"DataNumber":{"value":6414}},"city":{"DataString":{"value":"Oberarth"}}}}}</t>
-  </si>
-  <si>
     <t>Mapping Id (ident)</t>
   </si>
   <si>
     <t>address-mapping</t>
   </si>
   <si>
-    <t>{"ident":"address-mapping","formIdent":"address-form","dataIdent":"address-data","mappings":[{"formIdent":"TEXTFIELD-42","dataIdent":"street"},{"formIdent":"TEXTFIELD-14911","dataIdent":"number"},{"formIdent":"TEXTFIELD-33671","dataIdent":"postcode"},{"formIdent":"TEXTFIELD-90871","dataIdent":"city"}]}</t>
-  </si>
-  <si>
     <t>send-email</t>
   </si>
   <si>
     <t>{"ident":"send-email","elems":[{"ident":"ELEM-84079","elementType":"TITLE","texts":{"label":{"textType":"LABEL","texts":{"EN":"Send Email Task","DE":"Send Email Task"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"smtpConfig","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"SMTP Configuration","DE":"SMTP Konfiguration"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"default","required":false,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"subject","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Subject","DE":"Betreff"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"I18N Email Test-Subject: {{mail.info.subject}}!","required":true,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"content","elementType":"TEXTAREA","texts":{"label":{"textType":"LABEL","texts":{"EN":"Content","DE":"Inhalt"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"Guten Tag\n\nDies ist ein Test Email.\n\nFreundliche Grüsse\n\nBPF-Team","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"from","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"From (Sender)","DE":"Von (Sender)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Email Address of the Sender.","DE":"Email Adresse des Senders."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"sender@finnova.ch","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":true,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"to","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"To (Recipients)","DE":"To (Empfänger)"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Semicolon separated list of all recipient's email addresses .","DE":"Strichpunkt getrennte Liste aller Email-Adressen der Empfänger."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"hans.muster@test.com; vreny.mueller@test.com","required":true,"inline":false,"readOnly":false,"layoutWide":"EIGHT","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"ELEM-73603","elementType":"DIVIDER","texts":{"label":{"textType":"LABEL","texts":{"EN":"Additional Attributes for HTML Emails","DE":"Weitere Werte für die HTML Emails"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"SIZE_CLASS","value":"big"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"templName","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Name","DE":"Template Name"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"The name of the HTML Template File.","DE":"Der Name der HTML Template Date."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"info_mail.html","required":false,"inline":false,"readOnly":false,"layoutWide":"TEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"language","elementType":"DROPDOWN","texts":{"label":{"textType":"LABEL","texts":{"EN":"Language","DE":"Sprache"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"},{"extraProp":"CLEARABLE","value":"false"}]},"value":"DE","required":false,"inline":false,"readOnly":false,"layoutWide":"SIX","elemEntries":{"entries":[{"key":"DE","label":{"textType":"LABEL","texts":{"EN":"German","DE":"Deutsch"}},"ident":"ENTRY-3318"},{"key":"EN","label":{"textType":"LABEL","texts":{"EN":"English","DE":"Englisch"}},"ident":"ENTRY-3546"}]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"templParams","elementType":"TEXTAREA","texts":{"label":{"textType":"LABEL","texts":{"EN":"Template Parameters","DE":"Template Parameter"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"Parameters as a Map that are used in the Template.","DE":"Ein JSON-Objekt, mit den Parameter, welche dem Template mitgegeben werden."}}},"extras":{"propValues":[{"extraProp":"INPUT_TYPE","value":"text"},{"extraProp":"SIZE","value":"20"}]},"value":"{\n \"header\": \"Finnova rocks\",\n \"greeting\": \"Dear Mister President\",\n \"content\": \"Lory Logsi Dogsi Email content with Link: link:nextTask\",\n \"footer\": \"visit us!\",\n \"nextTask\": \"Go to next Task.\",\n \"nextTaskLink\": \"link:nextTask\",\n \"startInstance\": \"Start new Process Instance\",\n \"startInstanceLink\": \"link:startInstance\"\n }","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
   </si>
   <si>
-    <t>{"ident":"address-form","elems":[{"ident":"TITLE-60664","elementType":"TITLE","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[]}},{"ident":"street","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Sonnenweg","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"number","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"23a","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"postcode","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"number"}]},"value":"6414","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":9999}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"town","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Oberarth","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+    <t>{"ident":"address","elems":[{"ident":"TITLE-60664","elementType":"TITLE","texts":{"label":{"textType":"LABEL","texts":{"EN":"Address","DE":"Adresse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE_CLASS","value":"huge"}]},"value":"","required":false,"inline":false,"readOnly":false,"layoutWide":"SIXTEEN","elemEntries":{"entries":[]},"validations":{"rules":[]}},{"ident":"street","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Street","DE":"Strasse"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Sonnenweg","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"number","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Number","DE":"Nummer"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"23a","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"postcode","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Postcode","DE":"Plz"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"number"}]},"value":"6414","required":true,"inline":false,"readOnly":false,"layoutWide":"FOUR","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":true,"params":{"intParam1":1000,"intParam2":9999}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}},{"ident":"town","elementType":"TEXTFIELD","texts":{"label":{"textType":"LABEL","texts":{"EN":"Town","DE":"Ort"}},"placeholder":{"textType":"PLACEHOLDER","texts":{"EN":"","DE":""}},"tooltip":{"textType":"TOOLTIP","texts":{"EN":"","DE":""}}},"extras":{"propValues":[{"extraProp":"SIZE","value":"20"},{"extraProp":"INPUT_TYPE","value":"text"}]},"value":"Oberarth","required":true,"inline":false,"readOnly":false,"layoutWide":"TWELVE","elemEntries":{"entries":[]},"validations":{"rules":[{"validationType":"EMAIL","enabled":false,"params":{}},{"validationType":"INTEGER","enabled":false,"params":{"intParam1":0,"intParam2":100}},{"validationType":"REG_EXP","enabled":false,"params":{"stringParam":""}}]}}]}</t>
+  </si>
+  <si>
+    <t>{"ident":"address-data","structure":{"value":[["street",{"DataString":{"value":"Sonnenweg"}}],["number",{"DataString":{"value":"23a"}}],["postcode",{"DataNumber":{"value":6414}}],["town",{"DataString":{"value":"Oberarth"}}]]}}</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>{"ident":"address-mapping","formIdent":"address","dataIdent":"address-data","mappings":[{"formIdent":"street","dataIdent":"street"},{"formIdent":"number","dataIdent":"number"},{"formIdent":"postcode","dataIdent":"postcode"},{"formIdent":"town","dataIdent":"town"}]}</t>
   </si>
 </sst>
 </file>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73630E78-9998-5148-A4F5-0F74AED6B7AF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="170" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A2" zoomScale="170" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -661,26 +661,26 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -693,7 +693,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="170" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -704,18 +704,18 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A6BC9-3416-B348-8790-05B6BEA43B74}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -738,18 +738,18 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Json-View / removed Value form DataStructure
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC1B9D6-A197-9146-99B9-E15FC37F7D6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35ABF25-2C01-E64D-9EC9-FE2C054E42F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="17" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -151,13 +151,7 @@
     <t>{"ident":"address-mapping","formIdent":"address","dataIdent":"address-data","mappings":[{"formIdent":"street","dataIdent":"street"},{"formIdent":"number","dataIdent":"number"},{"formIdent":"postcode","dataIdent":"postcode"},{"formIdent":"town","dataIdent":"town"}]}</t>
   </si>
   <si>
-    <t>address-object-data</t>
-  </si>
-  <si>
-    <t>{"ident":"address-data","value":[{"DataString":{"ident":"street","value":"Sonnenweg"}},{"DataString":{"ident":"number","value":"23a"}},{"DataNumber":{"ident":"postcode","value":6414}},{"DataString":{"ident":"town","value":"Oberarth"}}]}</t>
-  </si>
-  <si>
-    <t>{"ident":"address-object-data","value":[{"DataObject":{"ident":"address","value":[{"DataString":{"ident":"number","value":"23a"}},{"DataNumber":{"ident":"postcode","value":6414}},{"DataString":{"ident":"town","value":"Oberarth"}},{"DataString":{"ident":"street","value":"Sonnenweg"}}]}}]}</t>
+    <t>{"ident":"address-data","children":[{"DataValue":{"ident":"street","structureType":"STRING"}},{"DataValue":{"ident":"number","structureType":"STRING"}},{"DataValue":{"ident":"postcode","structureType":"NUMBER"}},{"DataValue":{"ident":"town","structureType":"STRING"}}]}</t>
   </si>
 </sst>
 </file>
@@ -696,10 +690,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED31875-2B24-DD47-B72C-6F638FA3F984}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="170" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -721,15 +715,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -741,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A6BC9-3416-B348-8790-05B6BEA43B74}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added Cardinality / added resolver for resolution problem
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35ABF25-2C01-E64D-9EC9-FE2C054E42F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CB3D8E-C39C-6F40-BC12-6E78440F8CE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,14 +151,14 @@
     <t>{"ident":"address-mapping","formIdent":"address","dataIdent":"address-data","mappings":[{"formIdent":"street","dataIdent":"street"},{"formIdent":"number","dataIdent":"number"},{"formIdent":"postcode","dataIdent":"postcode"},{"formIdent":"town","dataIdent":"town"}]}</t>
   </si>
   <si>
-    <t>{"ident":"address-data","children":[{"DataValue":{"ident":"street","structureType":"STRING"}},{"DataValue":{"ident":"number","structureType":"STRING"}},{"DataValue":{"ident":"postcode","structureType":"NUMBER"}},{"DataValue":{"ident":"town","structureType":"STRING"}}]}</t>
+    <t>{"ident":"address-data","cardinality":"ONE","children":[{"DataValue":{"ident":"street","structureType":"STRING","cardinality":"ONE"}},{"DataValue":{"ident":"number","structureType":"STRING","cardinality":"ONE"}},{"DataValue":{"ident":"postcode","structureType":"NUMBER","cardinality":"ONE"}},{"DataValue":{"ident":"town","structureType":"STRING","cardinality":"ONE"}}]}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +180,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -214,11 +220,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +700,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScale="170" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -728,7 +735,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -744,11 +751,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Service Config - added persist and idents for Mocks
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CB3D8E-C39C-6F40-BC12-6E78440F8CE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3CA734-8BF7-D243-AEB9-5B78DD973E87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="17" r:id="rId1"/>
     <sheet name="forms" sheetId="18" r:id="rId2"/>
     <sheet name="data" sheetId="19" r:id="rId3"/>
     <sheet name="mappings" sheetId="20" r:id="rId4"/>
+    <sheet name="mocks" sheetId="21" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Username</t>
   </si>
@@ -152,6 +153,12 @@
   </si>
   <si>
     <t>{"ident":"address-data","cardinality":"ONE","children":[{"DataValue":{"ident":"street","structureType":"STRING","cardinality":"ONE"}},{"DataValue":{"ident":"number","structureType":"STRING","cardinality":"ONE"}},{"DataValue":{"ident":"postcode","structureType":"NUMBER","cardinality":"ONE"}},{"DataValue":{"ident":"town","structureType":"STRING","cardinality":"ONE"}}]}</t>
+  </si>
+  <si>
+    <t>swapi</t>
+  </si>
+  <si>
+    <t>{"ident":"swapi","mocks":[{"id":195,"url":"/api/people/{{peopleId}}","status":200,"content":"\n{\n\t\"name\": \"Luke Skywalker\",\n\t\"height\": \"172\",\n\t\"mass\": \"77\",\n\t\"hair_color\": \"blond\",\n\t\"skin_color\": \"fair\",\n\t\"eye_color\": \"blue\",\n\t\"birth_year\": \"19BBY\",\n\t\"gender\": \"male\",\n\t\"homeworld\": \"https://swapi.co/api/planets/1/\",\n\t\"films\": [\n\t\t\"https://swapi.co/api/films/2/\",\n\t\t\"https://swapi.co/api/films/6/\",\n\t\t\"https://swapi.co/api/films/3/\",\n\t\t\"https://swapi.co/api/films/1/\",\n\t\t\"https://swapi.co/api/films/7/\"\n\t],\n\t\"species\": [\n\t\t\"https://swapi.co/api/species/1/\"\n\t],\n\t\"vehicles\": [\n\t\t\"https://swapi.co/api/vehicles/14/\",\n\t\t\"https://swapi.co/api/vehicles/30/\"\n\t],\n\t\"starships\": [\n\t\t\"https://swapi.co/api/starships/12/\",\n\t\t\"https://swapi.co/api/starships/22/\"\n\t],\n\t\"created\": \"2014-12-09T13:50:51.644000Z\",\n\t\"edited\": \"2014-12-20T21:17:56.891000Z\",\n\t\"url\": \"https://swapi.co/api/people/1/\"\n}\n "},{"id":348,"url":"/api/films/2/","status":200,"content":"{\n \"title\" : \"The Empire Strikes Back\",\n \"episode_id\" : 5,\n \"opening_crawl\" : \"It is a dark time for the\\r\\nRebellion. Although the Death\\r\\nStar has been destroyed,\\r\\nImperial troops have driven the\\r\\nRebel forces from their hidden\\r\\nbase and pursued them across\\r\\nthe galaxy.\\r\\n\\r\\nEvading the dreaded Imperial\\r\\nStarfleet, a group of freedom\\r\\nfighters led by Luke Skywalker\\r\\nhas established a new secret\\r\\nbase on the remote ice world\\r\\nof Hoth.\\r\\n\\r\\nThe evil lord Darth Vader,\\r\\nobsessed with finding young\\r\\nSkywalker, has dispatched\\r\\nthousands of remote probes into\\r\\nthe far reaches of space....\",\n \"director\" : \"Irvin Kershner\",\n \"producer\" : \"Gary Kurtz, Rick McCallum\",\n \"release_date\" : \"1980-05-17\",\n \"characters\" : [ \"https://swapi.co/api/people/1/\", \"https://swapi.co/api/people/2/\", \"https://swapi.co/api/people/3/\", \"https://swapi.co/api/people/4/\", \"https://swapi.co/api/people/5/\", \"https://swapi.co/api/people/10/\", \"https://swapi.co/api/people/13/\", \"https://swapi.co/api/people/14/\", \"https://swapi.co/api/people/18/\", \"https://swapi.co/api/people/20/\", \"https://swapi.co/api/people/21/\", \"https://swapi.co/api/people/22/\", \"https://swapi.co/api/people/23/\", \"https://swapi.co/api/people/24/\", \"https://swapi.co/api/people/25/\", \"https://swapi.co/api/people/26/\" ],\n \"planets\" : [ \"https://swapi.co/api/planets/4/\", \"https://swapi.co/api/planets/5/\", \"https://swapi.co/api/planets/6/\", \"https://swapi.co/api/planets/27/\" ],\n \"starships\" : [ \"https://swapi.co/api/starships/15/\", \"https://swapi.co/api/starships/10/\", \"https://swapi.co/api/starships/11/\", \"https://swapi.co/api/starships/12/\", \"https://swapi.co/api/starships/21/\", \"https://swapi.co/api/starships/22/\", \"https://swapi.co/api/starships/23/\", \"https://swapi.co/api/starships/3/\", \"https://swapi.co/api/starships/17/\" ],\n \"vehicles\" : [ \"https://swapi.co/api/vehicles/8/\", \"https://swapi.co/api/vehicles/14/\", \"https://swapi.co/api/vehicles/16/\", \"https://swapi.co/api/vehicles/18/\", \"https://swapi.co/api/vehicles/19/\", \"https://swapi.co/api/vehicles/20/\" ],\n \"species\" : [ \"https://swapi.co/api/species/6/\", \"https://swapi.co/api/species/7/\", \"https://swapi.co/api/species/3/\", \"https://swapi.co/api/species/2/\", \"https://swapi.co/api/species/1/\" ],\n \"created\" : \"2014-12-12T11:26:24.656000Z\",\n \"edited\" : \"2017-04-19T10:57:29.544256Z\",\n \"url\" : \"https://swapi.co/api/films/2/\"\n}"},{"id":926,"url":"/api/vehicles/8/","status":200,"content":"{\n \"name\" : \"TIE/LN starfighter\",\n \"model\" : \"Twin Ion Engine/Ln Starfighter\",\n \"manufacturer\" : \"Sienar Fleet Systems\",\n \"cost_in_credits\" : \"unknown\",\n \"length\" : \"6.4\",\n \"max_atmosphering_speed\" : \"1200\",\n \"crew\" : \"1\",\n \"passengers\" : \"0\",\n \"cargo_capacity\" : \"65\",\n \"consumables\" : \"2 days\",\n \"vehicle_class\" : \"starfighter\",\n \"pilots\" : [ ],\n \"films\" : [ \"https://swapi.co/api/films/2/\", \"https://swapi.co/api/films/3/\", \"https://swapi.co/api/films/1/\" ],\n \"created\" : \"2014-12-10T16:33:52.860000Z\",\n \"edited\" : \"2014-12-22T18:21:15.606149Z\",\n \"url\" : \"https://swapi.co/api/vehicles/8/\"\n}"}]}</t>
   </si>
 </sst>
 </file>
@@ -699,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED31875-2B24-DD47-B72C-6F638FA3F984}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="170" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="170" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -734,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0A6BC9-3416-B348-8790-05B6BEA43B74}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -762,4 +769,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62CBF60-60ED-074D-8179-A38E8FE9B60D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added testing mock configurations.
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/pme123/play-binding-form/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3CA734-8BF7-D243-AEB9-5B78DD973E87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83085AD2-5F4F-6641-8D29-9F4956C41EE9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,7 +158,7 @@
     <t>swapi</t>
   </si>
   <si>
-    <t>{"ident":"swapi","mocks":[{"id":195,"url":"/api/people/{{peopleId}}","status":200,"content":"\n{\n\t\"name\": \"Luke Skywalker\",\n\t\"height\": \"172\",\n\t\"mass\": \"77\",\n\t\"hair_color\": \"blond\",\n\t\"skin_color\": \"fair\",\n\t\"eye_color\": \"blue\",\n\t\"birth_year\": \"19BBY\",\n\t\"gender\": \"male\",\n\t\"homeworld\": \"https://swapi.co/api/planets/1/\",\n\t\"films\": [\n\t\t\"https://swapi.co/api/films/2/\",\n\t\t\"https://swapi.co/api/films/6/\",\n\t\t\"https://swapi.co/api/films/3/\",\n\t\t\"https://swapi.co/api/films/1/\",\n\t\t\"https://swapi.co/api/films/7/\"\n\t],\n\t\"species\": [\n\t\t\"https://swapi.co/api/species/1/\"\n\t],\n\t\"vehicles\": [\n\t\t\"https://swapi.co/api/vehicles/14/\",\n\t\t\"https://swapi.co/api/vehicles/30/\"\n\t],\n\t\"starships\": [\n\t\t\"https://swapi.co/api/starships/12/\",\n\t\t\"https://swapi.co/api/starships/22/\"\n\t],\n\t\"created\": \"2014-12-09T13:50:51.644000Z\",\n\t\"edited\": \"2014-12-20T21:17:56.891000Z\",\n\t\"url\": \"https://swapi.co/api/people/1/\"\n}\n "},{"id":348,"url":"/api/films/2/","status":200,"content":"{\n \"title\" : \"The Empire Strikes Back\",\n \"episode_id\" : 5,\n \"opening_crawl\" : \"It is a dark time for the\\r\\nRebellion. Although the Death\\r\\nStar has been destroyed,\\r\\nImperial troops have driven the\\r\\nRebel forces from their hidden\\r\\nbase and pursued them across\\r\\nthe galaxy.\\r\\n\\r\\nEvading the dreaded Imperial\\r\\nStarfleet, a group of freedom\\r\\nfighters led by Luke Skywalker\\r\\nhas established a new secret\\r\\nbase on the remote ice world\\r\\nof Hoth.\\r\\n\\r\\nThe evil lord Darth Vader,\\r\\nobsessed with finding young\\r\\nSkywalker, has dispatched\\r\\nthousands of remote probes into\\r\\nthe far reaches of space....\",\n \"director\" : \"Irvin Kershner\",\n \"producer\" : \"Gary Kurtz, Rick McCallum\",\n \"release_date\" : \"1980-05-17\",\n \"characters\" : [ \"https://swapi.co/api/people/1/\", \"https://swapi.co/api/people/2/\", \"https://swapi.co/api/people/3/\", \"https://swapi.co/api/people/4/\", \"https://swapi.co/api/people/5/\", \"https://swapi.co/api/people/10/\", \"https://swapi.co/api/people/13/\", \"https://swapi.co/api/people/14/\", \"https://swapi.co/api/people/18/\", \"https://swapi.co/api/people/20/\", \"https://swapi.co/api/people/21/\", \"https://swapi.co/api/people/22/\", \"https://swapi.co/api/people/23/\", \"https://swapi.co/api/people/24/\", \"https://swapi.co/api/people/25/\", \"https://swapi.co/api/people/26/\" ],\n \"planets\" : [ \"https://swapi.co/api/planets/4/\", \"https://swapi.co/api/planets/5/\", \"https://swapi.co/api/planets/6/\", \"https://swapi.co/api/planets/27/\" ],\n \"starships\" : [ \"https://swapi.co/api/starships/15/\", \"https://swapi.co/api/starships/10/\", \"https://swapi.co/api/starships/11/\", \"https://swapi.co/api/starships/12/\", \"https://swapi.co/api/starships/21/\", \"https://swapi.co/api/starships/22/\", \"https://swapi.co/api/starships/23/\", \"https://swapi.co/api/starships/3/\", \"https://swapi.co/api/starships/17/\" ],\n \"vehicles\" : [ \"https://swapi.co/api/vehicles/8/\", \"https://swapi.co/api/vehicles/14/\", \"https://swapi.co/api/vehicles/16/\", \"https://swapi.co/api/vehicles/18/\", \"https://swapi.co/api/vehicles/19/\", \"https://swapi.co/api/vehicles/20/\" ],\n \"species\" : [ \"https://swapi.co/api/species/6/\", \"https://swapi.co/api/species/7/\", \"https://swapi.co/api/species/3/\", \"https://swapi.co/api/species/2/\", \"https://swapi.co/api/species/1/\" ],\n \"created\" : \"2014-12-12T11:26:24.656000Z\",\n \"edited\" : \"2017-04-19T10:57:29.544256Z\",\n \"url\" : \"https://swapi.co/api/films/2/\"\n}"},{"id":926,"url":"/api/vehicles/8/","status":200,"content":"{\n \"name\" : \"TIE/LN starfighter\",\n \"model\" : \"Twin Ion Engine/Ln Starfighter\",\n \"manufacturer\" : \"Sienar Fleet Systems\",\n \"cost_in_credits\" : \"unknown\",\n \"length\" : \"6.4\",\n \"max_atmosphering_speed\" : \"1200\",\n \"crew\" : \"1\",\n \"passengers\" : \"0\",\n \"cargo_capacity\" : \"65\",\n \"consumables\" : \"2 days\",\n \"vehicle_class\" : \"starfighter\",\n \"pilots\" : [ ],\n \"films\" : [ \"https://swapi.co/api/films/2/\", \"https://swapi.co/api/films/3/\", \"https://swapi.co/api/films/1/\" ],\n \"created\" : \"2014-12-10T16:33:52.860000Z\",\n \"edited\" : \"2014-12-22T18:21:15.606149Z\",\n \"url\" : \"https://swapi.co/api/vehicles/8/\"\n}"}]}</t>
+    <t>{"ident":"swapi","mocks":[{"id":195,"url":"api/people/{{peopleId}}","status":200,"content":"\n{\n\t\"name\": \"Luke Skywalker\",\n\t\"height\": \"172\",\n\t\"mass\": \"77\",\n\t\"hair_color\": \"blond\",\n\t\"skin_color\": \"fair\",\n\t\"eye_color\": \"blue\",\n\t\"birth_year\": \"19BBY\",\n\t\"gender\": \"male\",\n\t\"homeworld\": \"https://swapi.co/api/planets/1/\",\n\t\"films\": [\n\t\t\"https://swapi.co/api/films/2/\",\n\t\t\"https://swapi.co/api/films/6/\",\n\t\t\"https://swapi.co/api/films/3/\",\n\t\t\"https://swapi.co/api/films/1/\",\n\t\t\"https://swapi.co/api/films/7/\"\n\t],\n\t\"species\": [\n\t\t\"https://swapi.co/api/species/1/\"\n\t],\n\t\"vehicles\": [\n\t\t\"https://swapi.co/api/vehicles/14/\",\n\t\t\"https://swapi.co/api/vehicles/30/\"\n\t],\n\t\"starships\": [\n\t\t\"https://swapi.co/api/starships/12/\",\n\t\t\"https://swapi.co/api/starships/22/\"\n\t],\n\t\"created\": \"2014-12-09T13:50:51.644000Z\",\n\t\"edited\": \"2014-12-20T21:17:56.891000Z\",\n\t\"url\": \"https://swapi.co/api/people/{{peopleId}}/\"\n}\n "},{"id":348,"url":"api/films/{{filmId}}","status":200,"content":"{\n \"title\" : \"The Empire Strikes Back\",\n \"episode_id\" : 5,\n \"opening_crawl\" : \"It is a dark time for the\\r\\nRebellion. Although the Death\\r\\nStar has been destroyed,\\r\\nImperial troops have driven the\\r\\nRebel forces from their hidden\\r\\nbase and pursued them across\\r\\nthe galaxy.\\r\\n\\r\\nEvading the dreaded Imperial\\r\\nStarfleet, a group of freedom\\r\\nfighters led by Luke Skywalker\\r\\nhas established a new secret\\r\\nbase on the remote ice world\\r\\nof Hoth.\\r\\n\\r\\nThe evil lord Darth Vader,\\r\\nobsessed with finding young\\r\\nSkywalker, has dispatched\\r\\nthousands of remote probes into\\r\\nthe far reaches of space....\",\n \"director\" : \"Irvin Kershner\",\n \"producer\" : \"Gary Kurtz, Rick McCallum\",\n \"release_date\" : \"1980-05-17\",\n \"characters\" : [ \"https://swapi.co/api/people/1/\", \"https://swapi.co/api/people/2/\", \"https://swapi.co/api/people/3/\", \"https://swapi.co/api/people/4/\", \"https://swapi.co/api/people/5/\", \"https://swapi.co/api/people/10/\", \"https://swapi.co/api/people/13/\", \"https://swapi.co/api/people/14/\", \"https://swapi.co/api/people/18/\", \"https://swapi.co/api/people/20/\", \"https://swapi.co/api/people/21/\", \"https://swapi.co/api/people/22/\", \"https://swapi.co/api/people/23/\", \"https://swapi.co/api/people/24/\", \"https://swapi.co/api/people/25/\", \"https://swapi.co/api/people/26/\" ],\n \"planets\" : [ \"https://swapi.co/api/planets/4/\", \"https://swapi.co/api/planets/5/\", \"https://swapi.co/api/planets/6/\", \"https://swapi.co/api/planets/27/\" ],\n \"starships\" : [ \"https://swapi.co/api/starships/15/\", \"https://swapi.co/api/starships/10/\", \"https://swapi.co/api/starships/11/\", \"https://swapi.co/api/starships/12/\", \"https://swapi.co/api/starships/21/\", \"https://swapi.co/api/starships/22/\", \"https://swapi.co/api/starships/23/\", \"https://swapi.co/api/starships/3/\", \"https://swapi.co/api/starships/17/\" ],\n \"vehicles\" : [ \"https://swapi.co/api/vehicles/8/\", \"https://swapi.co/api/vehicles/14/\", \"https://swapi.co/api/vehicles/16/\", \"https://swapi.co/api/vehicles/18/\", \"https://swapi.co/api/vehicles/19/\", \"https://swapi.co/api/vehicles/20/\" ],\n \"species\" : [ \"https://swapi.co/api/species/6/\", \"https://swapi.co/api/species/7/\", \"https://swapi.co/api/species/3/\", \"https://swapi.co/api/species/2/\", \"https://swapi.co/api/species/1/\" ],\n \"created\" : \"2014-12-12T11:26:24.656000Z\",\n \"edited\" : \"2017-04-19T10:57:29.544256Z\",\n \"url\" : \"https://swapi.co/api/films/{{filmId}}/\"\n}"},{"id":926,"url":"api/vehicles/{{vehicleId}}","status":200,"content":"{\n \"name\" : \"TIE/LN starfighter\",\n \"model\" : \"Twin Ion Engine/Ln Starfighter\",\n \"manufacturer\" : \"Sienar Fleet Systems\",\n \"cost_in_credits\" : \"unknown\",\n \"length\" : \"6.4\",\n \"max_atmosphering_speed\" : \"1200\",\n \"crew\" : \"1\",\n \"passengers\" : \"0\",\n \"cargo_capacity\" : \"65\",\n \"consumables\" : \"2 days\",\n \"vehicle_class\" : \"starfighter\",\n \"pilots\" : [ ],\n \"films\" : [ \"https://swapi.co/api/films/2/\", \"https://swapi.co/api/films/3/\", \"https://swapi.co/api/films/1/\" ],\n \"created\" : \"2014-12-10T16:33:52.860000Z\",\n \"edited\" : \"2014-12-22T18:21:15.606149Z\",\n \"url\" : \"https://swapi.co/api/vehicles/{{vehicleId}}/\"\n}"}]}</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>